<commit_message>
atualizei a planilha de riscos
</commit_message>
<xml_diff>
--- a/documentação/Riscos.xlsx
+++ b/documentação/Riscos.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aluno\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yurih\Desktop\projeto pi\Projeto-Luminous-v-\documentação\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9FC521C9-0F57-42B7-A3D6-FDDEF16EB26E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{802877AB-2CF4-4B09-BA16-1A39106D57A4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{4012E409-80F3-444A-A65A-0C8982D78FFB}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>RISCOS</t>
   </si>
@@ -78,6 +78,18 @@
   </si>
   <si>
     <t>Manter todos os membros  Apresentar a parte do membro que não pode comparecer.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">         Manter o grupo todo atualizado com os requisitos pendentes e com as datas das entregas.</t>
+  </si>
+  <si>
+    <t>Fazer reunião emergencial, discutir metas pendentes e fazer a redivisão das tarefas.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Explicar tudo o que está a ser feito, manter o grupo alinhado em relação ao projeto e procurar ajuda dos membros </t>
+  </si>
+  <si>
+    <t>Dividir as atividades de acordo com as capacidades individuais dos integrantes do grupo</t>
   </si>
 </sst>
 </file>
@@ -173,7 +185,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -191,15 +203,11 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -517,8 +525,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43B6CF0E-0A43-4363-8DBD-E20F72A76353}">
   <dimension ref="C3:H22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -533,19 +541,19 @@
   </cols>
   <sheetData>
     <row r="3" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D3" s="8" t="s">
+      <c r="D3" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="E3" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="F3" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="G3" s="8" t="s">
+      <c r="F3" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="G3" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="H3" s="8" t="s">
+      <c r="H3" s="7" t="s">
         <v>11</v>
       </c>
     </row>
@@ -563,7 +571,7 @@
         <f>E4*F4</f>
         <v>4</v>
       </c>
-      <c r="H4" s="10" t="s">
+      <c r="H4" s="8" t="s">
         <v>12</v>
       </c>
     </row>
@@ -581,7 +589,7 @@
         <f t="shared" ref="G5:G10" si="0">E5*F5</f>
         <v>3</v>
       </c>
-      <c r="H5" s="9" t="s">
+      <c r="H5" s="8" t="s">
         <v>13</v>
       </c>
     </row>
@@ -599,7 +607,7 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="H6" s="9" t="s">
+      <c r="H6" s="8" t="s">
         <v>14</v>
       </c>
     </row>
@@ -617,7 +625,9 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="H7" s="7"/>
+      <c r="H7" s="8" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="8" spans="4:8" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D8" s="6" t="s">
@@ -633,7 +643,9 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="H8" s="7"/>
+      <c r="H8" s="8" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="9" spans="4:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D9" s="6" t="s">
@@ -649,7 +661,9 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="H9" s="7"/>
+      <c r="H9" s="8" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="10" spans="4:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D10" s="6" t="s">
@@ -665,7 +679,9 @@
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="H10" s="7"/>
+      <c r="H10" s="8" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="11" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D11" s="1"/>

</xml_diff>

<commit_message>
alterando a planilha de riscos
</commit_message>
<xml_diff>
--- a/documentação/Riscos.xlsx
+++ b/documentação/Riscos.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yurih\Desktop\projeto pi\Projeto-Luminous-v-\documentação\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luiss\Desktop\Projeto-Luminous-v-\documentação\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{802877AB-2CF4-4B09-BA16-1A39106D57A4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27DEC008-F4A3-4797-9045-690469893418}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{4012E409-80F3-444A-A65A-0C8982D78FFB}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{4012E409-80F3-444A-A65A-0C8982D78FFB}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="23">
   <si>
     <t>RISCOS</t>
   </si>
@@ -90,13 +90,25 @@
   </si>
   <si>
     <t>Dividir as atividades de acordo com as capacidades individuais dos integrantes do grupo</t>
+  </si>
+  <si>
+    <t>Solução</t>
+  </si>
+  <si>
+    <t>Mitigar</t>
+  </si>
+  <si>
+    <t>Evitar</t>
+  </si>
+  <si>
+    <t>Eliminar</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -119,8 +131,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFF00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -129,19 +149,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -153,12 +161,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF6600"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -181,33 +195,219 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -215,6 +415,13 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF05A40A"/>
+      <color rgb="FF5CA414"/>
+      <color rgb="FFFF6600"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -523,10 +730,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43B6CF0E-0A43-4363-8DBD-E20F72A76353}">
-  <dimension ref="C3:H22"/>
+  <dimension ref="C3:I22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4:I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -537,188 +744,213 @@
     <col min="5" max="5" width="16.42578125" customWidth="1"/>
     <col min="6" max="6" width="13.85546875" customWidth="1"/>
     <col min="7" max="7" width="13.140625" customWidth="1"/>
-    <col min="8" max="8" width="110.28515625" customWidth="1"/>
+    <col min="8" max="8" width="11.5703125" customWidth="1"/>
+    <col min="9" max="9" width="104.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D3" s="7" t="s">
+    <row r="3" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D3" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="E3" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="F3" s="7" t="s">
+      <c r="F3" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="G3" s="7" t="s">
+      <c r="G3" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="H3" s="7" t="s">
+      <c r="H3" s="16" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="4" spans="4:8" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D4" s="6" t="s">
+      <c r="I3" s="10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="4:9" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D4" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="4">
+      <c r="E4" s="3">
         <v>2</v>
       </c>
-      <c r="F4" s="4">
+      <c r="F4" s="3">
         <v>2</v>
       </c>
-      <c r="G4" s="3">
+      <c r="G4" s="2">
         <f>E4*F4</f>
         <v>4</v>
       </c>
-      <c r="H4" s="8" t="s">
+      <c r="H4" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="I4" s="9" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="4:8" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D5" s="6" t="s">
+    <row r="5" spans="4:9" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D5" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="E5" s="2">
+      <c r="E5" s="8">
         <v>1</v>
       </c>
-      <c r="F5" s="5">
+      <c r="F5" s="7">
         <v>3</v>
       </c>
-      <c r="G5" s="3">
+      <c r="G5" s="2">
         <f t="shared" ref="G5:G10" si="0">E5*F5</f>
         <v>3</v>
       </c>
-      <c r="H5" s="8" t="s">
+      <c r="H5" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="I5" s="13" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="4:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D6" s="6" t="s">
+    <row r="6" spans="4:9" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D6" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="E6" s="4">
+      <c r="E6" s="3">
         <v>2</v>
       </c>
-      <c r="F6" s="4">
+      <c r="F6" s="3">
         <v>2</v>
       </c>
-      <c r="G6" s="3">
+      <c r="G6" s="2">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="H6" s="8" t="s">
+      <c r="H6" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="I6" s="13" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="4:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D7" s="6" t="s">
+    <row r="7" spans="4:9" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D7" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="E7" s="4">
+      <c r="E7" s="3">
         <v>2</v>
       </c>
-      <c r="F7" s="5">
+      <c r="F7" s="7">
         <v>3</v>
       </c>
-      <c r="G7" s="3">
+      <c r="G7" s="2">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="H7" s="8" t="s">
+      <c r="H7" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="I7" s="13" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="4:8" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D8" s="6" t="s">
+    <row r="8" spans="4:9" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D8" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E8" s="4">
+      <c r="E8" s="3">
         <v>2</v>
       </c>
-      <c r="F8" s="4">
+      <c r="F8" s="3">
         <v>2</v>
       </c>
-      <c r="G8" s="3">
+      <c r="G8" s="2">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="H8" s="8" t="s">
+      <c r="H8" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="I8" s="13" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="4:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D9" s="6" t="s">
+    <row r="9" spans="4:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D9" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E9" s="4">
+      <c r="E9" s="3">
         <v>2</v>
       </c>
-      <c r="F9" s="5">
+      <c r="F9" s="7">
         <v>3</v>
       </c>
-      <c r="G9" s="3">
+      <c r="G9" s="2">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="H9" s="8" t="s">
+      <c r="H9" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="I9" s="13" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="4:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="4:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D10" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="E10" s="4">
+      <c r="E10" s="3">
         <v>3</v>
       </c>
-      <c r="F10" s="4">
+      <c r="F10" s="3">
         <v>3</v>
       </c>
-      <c r="G10" s="3">
+      <c r="G10" s="7">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="H10" s="8" t="s">
+      <c r="H10" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="I10" s="13" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
     </row>
-    <row r="12" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D12" s="1"/>
+    <row r="12" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D12" s="4"/>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
     </row>
-    <row r="13" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
     </row>
-    <row r="14" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
     </row>
-    <row r="15" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
     </row>
-    <row r="16" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>

</xml_diff>